<commit_message>
fix: validation of acquisitions files
</commit_message>
<xml_diff>
--- a/parameters_result.xlsx
+++ b/parameters_result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,651 +748,1004 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>22528025</t>
+          <t>21281662</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9885468955905812</v>
-      </c>
-      <c r="C13" t="n">
-        <v>6.624206720765709e-05</v>
+        <v>0.9997031464334705</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="D13" t="n">
-        <v>0.999999866011401</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.9980044446460157</v>
+        <v>0.9999998660010492</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="F13" t="n">
-        <v>0.9775630411951303</v>
-      </c>
-      <c r="G13" t="n">
-        <v>6.550604423868313e-05</v>
+        <v>0.9997031464334705</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>24259471</t>
+          <t>22528025</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9987777563443073</v>
+        <v>0.9885468955905812</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0005762924382716049</v>
+        <v>6.624206720765709e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9999998658768962</v>
+        <v>0.999999866011401</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9997676039972112</v>
+        <v>0.9980044446460157</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9987777563443073</v>
+        <v>0.9775630411951303</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0005762924382716049</v>
+        <v>6.550604423868313e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>24780201</t>
+          <t>24259471</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9992728695130315</v>
+        <v>0.9987777563443073</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0002176836848422497</v>
+        <v>0.0005762924382716049</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9999998659433507</v>
+        <v>0.9999998658768962</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9993849938499385</v>
+        <v>0.9997676039972112</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9992728695130315</v>
+        <v>0.9987777563443073</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0002176836848422497</v>
+        <v>0.0005762924382716049</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>26444330</t>
+          <t>24780201</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9997602130486969</v>
+        <v>0.9992728695130315</v>
       </c>
       <c r="C16" t="n">
-        <v>0.000147355109739369</v>
+        <v>0.0002176836848422497</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9999998660086979</v>
+        <v>0.9999998659433507</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9990917347865577</v>
+        <v>0.9993849938499385</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9997602130486969</v>
+        <v>0.9992728695130315</v>
       </c>
       <c r="G16" t="n">
-        <v>0.000147355109739369</v>
+        <v>0.0002176836848422497</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>26618355</t>
+          <t>26444330</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9988310721021948</v>
+        <v>0.9997602130486969</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0002534507887517147</v>
+        <v>0.000147355109739369</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9999998658840554</v>
+        <v>0.9999998660086979</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9994717379820391</v>
+        <v>0.9990917347865577</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9988310721021948</v>
+        <v>0.9997602130486969</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0002534507887517147</v>
+        <v>0.000147355109739369</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>27040152</t>
+          <t>26618355</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9999232413837449</v>
+        <v>0.9988310721021948</v>
       </c>
       <c r="C18" t="n">
-        <v>4.166130829903978e-05</v>
+        <v>0.0002534507887517147</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9999998660305439</v>
+        <v>0.9999998658840554</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9967948717948718</v>
+        <v>0.9994717379820391</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9999232413837449</v>
+        <v>0.9988310721021948</v>
       </c>
       <c r="G18" t="n">
-        <v>4.166130829903978e-05</v>
+        <v>0.0002534507887517147</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>27708269</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.9995492273233882</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0001419967421124828</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.9999998659804149</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.9990574929311969</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.9995492273233882</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.0001419967421124828</v>
+          <t>26731283</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>27812007</t>
+          <t>27040152</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9998744802383402</v>
+        <v>0.9999232413837449</v>
       </c>
       <c r="C20" t="n">
-        <v>4.742155349794238e-05</v>
+        <v>4.166130829903978e-05</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9999998660240106</v>
+        <v>0.9999998660305439</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9971830985915493</v>
+        <v>0.9967948717948718</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9998744802383402</v>
+        <v>0.9999232413837449</v>
       </c>
       <c r="G20" t="n">
-        <v>4.742155349794238e-05</v>
+        <v>4.166130829903978e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>27881548</t>
+          <t>27130020</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9998139306841564</v>
-      </c>
-      <c r="C21" t="n">
-        <v>7.595486111111111e-05</v>
+        <v>0.9997363683127573</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="D21" t="n">
-        <v>0.999999866015897</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.9982394366197183</v>
+        <v>0.9999998660055021</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="F21" t="n">
-        <v>0.9998139306841564</v>
-      </c>
-      <c r="G21" t="n">
-        <v>7.595486111111111e-05</v>
+        <v>0.9997363683127573</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30114957</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.9984563882458848</v>
+          <t>27434240</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
       </c>
       <c r="C22" t="n">
-        <v>0.0003331565072016461</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.9999998658337267</v>
+        <v>0.9999134623628257</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
       </c>
       <c r="E22" t="n">
-        <v>0.9995980707395499</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.9984563882458848</v>
+        <v>0.9999998660292337</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
       </c>
       <c r="G22" t="n">
-        <v>0.0003331565072016461</v>
+        <v>0.9999134623628257</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30345002</t>
+          <t>27708269</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9997722693758574</v>
+        <v>0.9995492273233882</v>
       </c>
       <c r="C23" t="n">
-        <v>8.171510631001372e-05</v>
+        <v>0.0001419967421124828</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9999998660103138</v>
+        <v>0.9999998659804149</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9983633387888707</v>
+        <v>0.9990574929311969</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9997722693758574</v>
+        <v>0.9995492273233882</v>
       </c>
       <c r="G23" t="n">
-        <v>8.171510631001372e-05</v>
+        <v>0.0001419967421124828</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>30401069</t>
+          <t>27812007</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9970834405006859</v>
+        <v>0.9998744802383402</v>
       </c>
       <c r="C24" t="n">
-        <v>0.001188084062071331</v>
+        <v>4.742155349794238e-05</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9999998656489846</v>
+        <v>0.9999998660240106</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9998872604284104</v>
+        <v>0.9971830985915493</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9970834405006859</v>
+        <v>0.9998744802383402</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001188084062071331</v>
+        <v>4.742155349794238e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>30860845</t>
+          <t>27881548</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.998959271047668</v>
+        <v>0.9998139306841564</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0006405928497942387</v>
+        <v>7.595486111111111e-05</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9999998659012669</v>
+        <v>0.999999866015897</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9997909261969475</v>
+        <v>0.9982394366197183</v>
       </c>
       <c r="F25" t="n">
-        <v>0.998959271047668</v>
+        <v>0.9998139306841564</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0006405928497942387</v>
+        <v>7.595486111111111e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>30974620</t>
+          <t>30114957</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9991059563614541</v>
+        <v>0.9984563882458848</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0003460165895061728</v>
+        <v>0.0003331565072016461</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9999998659209548</v>
+        <v>0.9999998658337267</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9996130030959752</v>
+        <v>0.9995980707395499</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9991059563614541</v>
+        <v>0.9984563882458848</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0003460165895061728</v>
+        <v>0.0003331565072016461</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>33068573</t>
+          <t>30345002</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9997498981910151</v>
+        <v>0.9997722693758574</v>
       </c>
       <c r="C27" t="n">
-        <v>9.712041323731139e-05</v>
+        <v>8.171510631001372e-05</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9999998660073155</v>
+        <v>0.9999998660103138</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9986225895316805</v>
+        <v>0.9983633387888707</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9997498981910151</v>
+        <v>0.9997722693758574</v>
       </c>
       <c r="G27" t="n">
-        <v>9.712041323731139e-05</v>
+        <v>8.171510631001372e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>33212135</t>
+          <t>30385373</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.9983938293038409</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.0005513760288065844</v>
+        <v>0.9997663751714677</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="D28" t="n">
-        <v>0.9999998658253199</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.9997571046878795</v>
+        <v>0.9999998660095237</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="F28" t="n">
-        <v>0.9983938293038409</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.0005513760288065844</v>
+        <v>0.9997663751714677</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>33604980</t>
+          <t>30401069</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.9999018079132374</v>
+        <v>0.9970834405006859</v>
       </c>
       <c r="C29" t="n">
-        <v>3.69727366255144e-05</v>
+        <v>0.001188084062071331</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9999998660276722</v>
+        <v>0.9999998656489846</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9963898916967509</v>
+        <v>0.9998872604284104</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9999018079132374</v>
+        <v>0.9970834405006859</v>
       </c>
       <c r="G29" t="n">
-        <v>3.69727366255144e-05</v>
+        <v>0.001188084062071331</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>33637942</t>
+          <t>30860845</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.9996681830847051</v>
+        <v>0.998959271047668</v>
       </c>
       <c r="C30" t="n">
-        <v>5.746849279835391e-05</v>
+        <v>0.0006405928497942387</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9999998659963626</v>
+        <v>0.9999998659012669</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9976744186046511</v>
+        <v>0.9997909261969475</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9996681830847051</v>
+        <v>0.998959271047668</v>
       </c>
       <c r="G30" t="n">
-        <v>5.746849279835391e-05</v>
+        <v>0.0006405928497942387</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>33773692</t>
+          <t>30974620</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.9997216328017833</v>
+        <v>0.9991059563614541</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0001332893947187929</v>
+        <v>0.0003460165895061728</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9999998660035271</v>
+        <v>0.9999998659209548</v>
       </c>
       <c r="E31" t="n">
-        <v>0.998995983935743</v>
+        <v>0.9996130030959752</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9997216328017833</v>
+        <v>0.9991059563614541</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0001332893947187929</v>
+        <v>0.0003460165895061728</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>33900783</t>
+          <t>33068573</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.9997579357424554</v>
+        <v>0.9997498981910151</v>
       </c>
       <c r="C32" t="n">
-        <v>8.640367798353909e-05</v>
+        <v>9.712041323731139e-05</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9999998660083927</v>
+        <v>0.9999998660073155</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9984520123839009</v>
+        <v>0.9986225895316805</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9997579357424554</v>
+        <v>0.9997498981910151</v>
       </c>
       <c r="G32" t="n">
-        <v>8.640367798353909e-05</v>
+        <v>9.712041323731139e-05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>33915934</t>
+          <t>33212135</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.9995494952417695</v>
+        <v>0.9983938293038409</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0001565982938957476</v>
+        <v>0.0005513760288065844</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9999998659804509</v>
+        <v>0.9999998658253199</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9991452991452991</v>
+        <v>0.9997571046878795</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9995494952417695</v>
+        <v>0.9983938293038409</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0001565982938957476</v>
+        <v>0.0005513760288065844</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>34393044</t>
+          <t>33275889</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.9996369705932785</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.0001121238425925926</v>
+        <v>0.9998645672582305</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="D34" t="n">
-        <v>0.9999998659921785</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.9988066825775657</v>
+        <v>0.9999998660226823</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="F34" t="n">
-        <v>0.9996369705932785</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.0001121238425925926</v>
+        <v>0.9998645672582305</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>34674493</t>
+          <t>33327331</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.9996668434927983</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.0001690564986282579</v>
+        <v>0.9997912915809328</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="D35" t="n">
-        <v>0.9999998659961831</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.9992082343626286</v>
+        <v>0.9999998660128631</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
       <c r="F35" t="n">
-        <v>0.9996668434927983</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.0001690564986282579</v>
+        <v>0.9997912915809328</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>35541276</t>
+          <t>33604980</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.9984850555126886</v>
+        <v>0.9999018079132374</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0004411276148834019</v>
+        <v>3.69727366255144e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>0.9999998658375787</v>
+        <v>0.9999998660276722</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9996964177292046</v>
+        <v>0.9963898916967509</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9984850555126886</v>
+        <v>0.9999018079132374</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0004411276148834019</v>
+        <v>3.69727366255144e-05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>36658002</t>
+          <t>33637942</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.9986700531550069</v>
+        <v>0.9996681830847051</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0002987289951989026</v>
+        <v>5.746849279835391e-05</v>
       </c>
       <c r="D37" t="n">
-        <v>0.9999998658624315</v>
+        <v>0.9999998659963626</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9995517705064993</v>
+        <v>0.9976744186046511</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9986700531550069</v>
+        <v>0.9996681830847051</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0002987289951989026</v>
+        <v>5.746849279835391e-05</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>33773692</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.9997216328017833</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0001332893947187929</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.9999998660035271</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.998995983935743</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.9997216328017833</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.0001332893947187929</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>33900783</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.9997579357424554</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8.640367798353909e-05</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.9999998660083927</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.9984520123839009</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.9997579357424554</v>
+      </c>
+      <c r="G39" t="n">
+        <v>8.640367798353909e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>33915934</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.9995494952417695</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0001565982938957476</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.9999998659804509</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9991452991452991</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.9995494952417695</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.0001565982938957476</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>34393044</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.9996369705932785</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0001121238425925926</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.9999998659921785</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.9988066825775657</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.9996369705932785</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0001121238425925926</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>34674493</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.9996668434927983</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.0001690564986282579</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9999998659961831</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.9992082343626286</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.9996668434927983</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.0001690564986282579</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>35541276</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.9984850555126886</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0004411276148834019</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9999998658375787</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.9996964177292046</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.9984850555126886</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.0004411276148834019</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>36658002</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.9986700531550069</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0002987289951989026</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9999998658624315</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.9995517705064993</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.9986700531550069</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.0002987289951989026</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>36961015</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.9997249817815501</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9999998660039759</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0.9997249817815501</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>37252590</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.9998877421982167</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9999998660257876</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0.9998877421982167</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>37467405</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>acquisition_2 no existe</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>37580279</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B48" t="n">
         <v>0.9999279299554183</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C48" t="n">
         <v>1.312800068587106e-05</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D48" t="n">
         <v>0.9999998660311721</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E48" t="n">
         <v>0.9898989898989899</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F48" t="n">
         <v>0.9999279299554183</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G48" t="n">
         <v>1.312800068587106e-05</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>37764949</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.9998625578703704</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.9999998660224131</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>0.9998625578703704</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>acquisition_3 no existe</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>